<commit_message>
Implementation of preloaded data
</commit_message>
<xml_diff>
--- a/src/assets/sample_files/preloadedData.xlsx
+++ b/src/assets/sample_files/preloadedData.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="126">
+  <si>
+    <t>Id</t>
+  </si>
   <si>
     <t>cName</t>
   </si>
@@ -58,73 +61,977 @@
     <t>yUrl</t>
   </si>
   <si>
-    <t>NodeJs</t>
-  </si>
-  <si>
-    <t>Mike Cantelon, Marc Harter, T.J. Holowaychuk, Nathan Rajlich</t>
-  </si>
-  <si>
-    <t>Manning Publications</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Node.js in Action</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>NodeJs</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Mike Cantelon, Marc Harter, T.J. Holowaychuk, Nathan Rajlich</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Manning Publications</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Node.js in Action</t>
+    </r>
   </si>
   <si>
     <t>https://www.manning.com/books/node-js-in-action</t>
   </si>
   <si>
-    <t xml:space="preserve"> Node.js - The Complete Guide (MVC, REST APIs, GraphQL, Deno)</t>
-  </si>
-  <si>
-    <t>Learn Node.js from scratch and build fully functional web applications. Covers topics like MVC architecture, REST APIs, GraphQL, Deno, and more.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Node.js - The Complete Guide (MVC, REST APIs, GraphQL, Deno)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Learn Node.js from scratch and build fully functional web applications. Covers topics like MVC architecture, REST APIs, GraphQL, Deno, and more.</t>
+    </r>
   </si>
   <si>
     <t>https://www.udemy.com/course/nodejs-the-complete-guide/</t>
   </si>
   <si>
-    <t>Udemy</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Udemy</t>
+    </r>
   </si>
   <si>
     <t>https://example.com/course-image.jpg</t>
   </si>
   <si>
-    <t>Programming with Mosh</t>
-  </si>
-  <si>
-    <t>A YouTube channel with Java tutorials for beginners and intermediate learners.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Programming with Mosh</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>A YouTube channel with Java tutorials for beginners and intermediate learners.</t>
+    </r>
   </si>
   <si>
     <t>https://www.youtube.com/programmingwithmosh</t>
   </si>
   <si>
-    <t>Marc Wandschneider</t>
-  </si>
-  <si>
-    <t>Addison-Wesley Professional</t>
-  </si>
-  <si>
-    <t>Learning Node.js: A Hands-On Guide to Building Web Applications in JavaScript</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Marc Wandschneider</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Addison-Wesley Professional</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Learning Node.js: A Hands-On Guide to Building Web Applications in JavaScript</t>
+    </r>
   </si>
   <si>
     <t>https://www.amazon.com/Learning-Node-js-Hands-Applications-JavaScript/dp/0321910575</t>
   </si>
   <si>
-    <t>The Complete Node.js Developer Course</t>
-  </si>
-  <si>
-    <t>A comprehensive course covering Node.js fundamentals, asynchronous programming, web development, and more</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>The Complete Node.js Developer Course</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>A comprehensive course covering Node.js fundamentals, asynchronous programming, web development, and more</t>
+    </r>
   </si>
   <si>
     <t>https://www.udemy.com/course/the-complete-nodejs-developer-course/</t>
   </si>
   <si>
-    <t>TheNewBoston</t>
-  </si>
-  <si>
-    <t>A YouTube channel with a comprehensive Java tutorial series.</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>TheNewBoston</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>A YouTube channel with a comprehensive Java tutorial series.</t>
+    </r>
   </si>
   <si>
     <t>https://www.youtube.com/thenewboston</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Java</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Herbert Schildt</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>McGraw-Hill Education</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>ava: The Complete Reference</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.example.com/java-complete-reference</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Java Programming Masterclass for Software Developers</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Comprehensive Java course on Udemy for beginners and experienced programmers.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/java-the-complete-java-developer-course</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>udemy</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Java Tutorial for Beginners</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>A step-by-step tutorial series for Java beginners by Telusko</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=IJquEga4-SY</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>java</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Cay S. Horstmann</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Wiley</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Core Java Volume I--Fundamentals</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.example.com/core-java-fundamentals</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Java In-Depth: Become a Complete Java Engineer!</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>A detailed Java course covering core concepts and advanced topics.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/java-in-depth-become-a-complete-java-engineer</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Programming with Mosh: Java Tutorial for Beginners</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Mosh Hamedani's Java tutorial series for beginners</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=eIrMbAQSU34</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>.Net</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Andrew Troelsen</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Apress</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Pro C# 8 with .NET Core 3: Foundational Principles and Practices in Programming</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.example.com/pro-c-sharp-dotnet-core</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>C# Basics for Beginners</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>A beginner-friendly course on Udemy to learn C# programming</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/csharp-tutorial-for-beginners</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>C# Fundamentals for Absolute Beginners</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Microsoft's official tutorial series for beginners to learn C# programming</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=gfkTfcpWqAY</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Adam Freeman</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Pro ASP.NET Core 5: Develop Cloud-Ready Web Applications Using MVC, Blazor, and Razor Pages</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.example.com/pro-aspnet-core</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>".NET Core 3.1 MVC and Razor Pages for Beginners</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Learn to build web applications using .NET Core MVC and Razor Pages</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/dotnet-core-mvc-for-beginners</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Traversy Media: .NET Core 5 MVC Crash Course</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>A crash course on building web applications with .NET Core MVC</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=C5cnZ-gZy2I</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Python</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Mark Lutz</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>O'Reilly Media</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Learning Python</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.example.com/learning-python</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Complete Python Bootcamp: Go from zero to hero in Python 3</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>A comprehensive Python course on Udemy for beginners and intermediate learners</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/complete-python-bootcamp</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Udemy</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Python Programming Tutorial for Beginners</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>A comprehensive Python tutorial series for beginners by Corey Schafer.",</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=_Z1a_9sdu4I</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Eric Matthes</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>No Starch Press</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Python Crash Course</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>https://www.example.com/python-crash-course"</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Python for Data Science and Machine Learning Bootcamp</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Learn Python for data analysis, visualization, and machine learning</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/python-for-data-science-and-machine-learning-bootcamp</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Sentdex: Python Programming for Finance</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Learn Python programming for financial analysis and algorithmic trading.",</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=2BrpKpWwT2A</t>
+  </si>
+  <si>
+    <t>Communication Skills</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Dale Carnegie</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Pocket Books</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>How to Win Friends and Influence People</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.example.com/how-to-win-friends</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Effective Communication Skills</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>A comprehensive online course to improve your communication skills.",</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.udemy.com/course/effective-communication-skills-course</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Improve Your Communication Skills: Speak with Confidence</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Tips and techniques to enhance your communication skills by Vanessa Van Edwards.",</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=6WwTakingUE</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Communication Skills</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Julian Treasure</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Penguin Books</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>How to be Heard: Secrets for Powerful Speaking and Listening</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.example.com/how-to-be-heard</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Public Speaking and Presentation Skills</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Learn how to confidently speak and present in front of an audience.",</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.coursera.org/specializations/public-speaking</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Coursera</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>TEDTalks: The Skill of Self-Confidence</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+      </rPr>
+      <t>Dr. Ivan Joseph discusses the skill of self-confidence and effective communication</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=w-HYZv6HzAs</t>
   </si>
 </sst>
 </file>
@@ -137,7 +1044,7 @@
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="29">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -164,16 +1071,50 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -312,8 +1253,14 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -322,6 +1269,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -507,7 +1460,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -528,6 +1481,19 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -631,170 +1597,190 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="6" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1057,242 +2043,588 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:N12"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6296296296296" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="2" max="2" width="33.7777777777778" customWidth="1"/>
-    <col min="3" max="3" width="20" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.7222222222222" customWidth="1"/>
-    <col min="5" max="5" width="22.1111111111111" style="1" customWidth="1"/>
-    <col min="6" max="6" width="50" style="1" customWidth="1"/>
-    <col min="7" max="7" width="23.5555555555556" customWidth="1"/>
-    <col min="8" max="8" width="62.7777777777778" style="1" customWidth="1"/>
-    <col min="9" max="9" width="35.3333333333333" customWidth="1"/>
-    <col min="11" max="11" width="33.1111111111111" customWidth="1"/>
-    <col min="12" max="12" width="21" style="1" customWidth="1"/>
-    <col min="13" max="13" width="35.8888888888889" style="1" customWidth="1"/>
-    <col min="14" max="14" width="23.4444444444444" style="1" customWidth="1"/>
+    <col min="1" max="1" width="7.84259259259259" customWidth="1"/>
+    <col min="2" max="2" width="29.2777777777778" customWidth="1"/>
+    <col min="3" max="3" width="33.7777777777778" customWidth="1"/>
+    <col min="4" max="4" width="20" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.7222222222222" customWidth="1"/>
+    <col min="6" max="6" width="22.1111111111111" style="2" customWidth="1"/>
+    <col min="7" max="7" width="50" style="2" customWidth="1"/>
+    <col min="8" max="8" width="23.5555555555556" customWidth="1"/>
+    <col min="9" max="9" width="62.7777777777778" style="2" customWidth="1"/>
+    <col min="10" max="10" width="35.3333333333333" customWidth="1"/>
+    <col min="12" max="12" width="33.1111111111111" customWidth="1"/>
+    <col min="13" max="13" width="21" style="2" customWidth="1"/>
+    <col min="14" max="14" width="35.8888888888889" style="2" customWidth="1"/>
+    <col min="15" max="15" width="23.4444444444444" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customHeight="1" spans="1:14">
-      <c r="A1" s="2" t="s">
+    <row r="1" customHeight="1" spans="1:15">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="6" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" customFormat="1" ht="39.6" spans="1:14">
-      <c r="A2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="5" t="s">
+    <row r="2" s="1" customFormat="1" ht="39.6" spans="1:15">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="8">
         <v>2014</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="7" t="s">
         <v>26</v>
       </c>
+      <c r="O2" s="9" t="s">
+        <v>27</v>
+      </c>
     </row>
-    <row r="3" customFormat="1" ht="52.8" spans="1:14">
-      <c r="A3" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" s="5" t="s">
+    <row r="3" s="1" customFormat="1" ht="52.8" spans="1:15">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="8">
         <v>2013</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="G3" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="J3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="K3" s="6" t="s">
+      <c r="J3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="L3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="M3" s="5" t="s">
+      <c r="L3" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="M3" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="N3" s="6" t="s">
+      <c r="N3" s="7" t="s">
         <v>36</v>
       </c>
+      <c r="O3" s="9" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="4" customFormat="1" customHeight="1" spans="5:14">
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="L4" s="1"/>
-      <c r="M4" s="1"/>
-      <c r="N4" s="1"/>
+    <row r="4" s="1" customFormat="1" ht="41.4" spans="1:15">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="10">
+        <v>2017</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="N4" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="O4" s="13" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="5" customFormat="1" customHeight="1" spans="5:14">
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
+    <row r="5" s="1" customFormat="1" ht="43.2" spans="1:15">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="10">
+        <v>2020</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="J5" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="K5" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="L5" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="O5" s="13" t="s">
+        <v>60</v>
+      </c>
     </row>
-    <row r="6" customFormat="1" customHeight="1" spans="5:14">
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="H6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="M6" s="1"/>
-      <c r="N6" s="1"/>
+    <row r="6" s="1" customFormat="1" ht="57.6" spans="1:15">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>62</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="12">
+        <v>2020</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="J6" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="L6" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="N6" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="O6" s="13" t="s">
+        <v>71</v>
+      </c>
     </row>
-    <row r="7" customFormat="1" customHeight="1" spans="5:14">
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="H7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
+    <row r="7" s="1" customFormat="1" ht="72" spans="1:15">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="12">
+        <v>2021</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="N7" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="O7" s="13" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="8" customFormat="1" customHeight="1" spans="5:14">
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
-      <c r="N8" s="1"/>
+    <row r="8" s="1" customFormat="1" ht="43.2" spans="1:15">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E8" s="12">
+        <v>2019</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="J8" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="L8" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="M8" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="N8" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="O8" s="13" t="s">
+        <v>92</v>
+      </c>
     </row>
-    <row r="9" customFormat="1" customHeight="1" spans="5:14">
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
+    <row r="9" s="1" customFormat="1" ht="43.2" spans="1:15">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="E9" s="12">
+        <v>2019</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="G9" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="H9" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="I9" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="J9" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="K9" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="L9" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="M9" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="N9" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="O9" s="13" t="s">
+        <v>102</v>
+      </c>
     </row>
-    <row r="10" customFormat="1" customHeight="1" spans="5:14">
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
+    <row r="10" s="1" customFormat="1" ht="43.2" spans="1:15">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="E10" s="12">
+        <v>1990</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="J10" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="K10" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="L10" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="M10" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="N10" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="O10" s="13" t="s">
+        <v>113</v>
+      </c>
     </row>
-    <row r="11" customFormat="1" customHeight="1" spans="5:14">
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
-      <c r="N11" s="1"/>
-    </row>
-    <row r="12" customFormat="1" customHeight="1" spans="5:14">
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
-      <c r="N12" s="1"/>
+    <row r="11" s="1" customFormat="1" ht="43.2" spans="1:15">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="E11" s="12">
+        <v>2017</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="H11" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="K11" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="L11" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="M11" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="N11" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="O11" s="13" t="s">
+        <v>125</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="https://www.manning.com/books/node-js-in-action"/>
-    <hyperlink ref="F3" r:id="rId2" display="https://www.amazon.com/Learning-Node-js-Hands-Applications-JavaScript/dp/0321910575"/>
-    <hyperlink ref="I2" r:id="rId3" display="https://www.udemy.com/course/nodejs-the-complete-guide/"/>
-    <hyperlink ref="K2" r:id="rId4" display="https://example.com/course-image.jpg"/>
-    <hyperlink ref="I3" r:id="rId5" display="https://www.udemy.com/course/the-complete-nodejs-developer-course/"/>
-    <hyperlink ref="K3" r:id="rId4" display="https://example.com/course-image.jpg"/>
-    <hyperlink ref="N2" r:id="rId6" display="https://www.youtube.com/programmingwithmosh"/>
-    <hyperlink ref="N3" r:id="rId7" display="https://www.youtube.com/thenewboston"/>
+    <hyperlink ref="G2" r:id="rId1" display="https://www.manning.com/books/node-js-in-action" tooltip="https://www.manning.com/books/node-js-in-action"/>
+    <hyperlink ref="J2" r:id="rId2" display="https://www.udemy.com/course/nodejs-the-complete-guide/" tooltip="https://www.udemy.com/course/nodejs-the-complete-guide/"/>
+    <hyperlink ref="L2" r:id="rId3" display="https://example.com/course-image.jpg" tooltip="https://example.com/course-image.jpg"/>
+    <hyperlink ref="O2" r:id="rId4" display="https://www.youtube.com/programmingwithmosh" tooltip="https://www.youtube.com/programmingwithmosh"/>
+    <hyperlink ref="G3" r:id="rId5" display="https://www.amazon.com/Learning-Node-js-Hands-Applications-JavaScript/dp/0321910575" tooltip="https://www.amazon.com/Learning-Node-js-Hands-Applications-JavaScript/dp/0321910575"/>
+    <hyperlink ref="J3" r:id="rId6" display="https://www.udemy.com/course/the-complete-nodejs-developer-course/" tooltip="https://www.udemy.com/course/the-complete-nodejs-developer-course/"/>
+    <hyperlink ref="L3" r:id="rId3" display="https://example.com/course-image.jpg" tooltip="https://example.com/course-image.jpg"/>
+    <hyperlink ref="O3" r:id="rId7" display="https://www.youtube.com/thenewboston" tooltip="https://www.youtube.com/thenewboston"/>
+    <hyperlink ref="G4" r:id="rId8" display="https://www.example.com/java-complete-reference" tooltip="https://www.example.com/java-complete-reference"/>
+    <hyperlink ref="J4" r:id="rId9" display="https://www.udemy.com/course/java-the-complete-java-developer-course" tooltip="https://www.udemy.com/course/java-the-complete-java-developer-course"/>
+    <hyperlink ref="L4" r:id="rId3" display="https://example.com/course-image.jpg" tooltip="https://example.com/course-image.jpg"/>
+    <hyperlink ref="O4" r:id="rId10" display="https://www.youtube.com/watch?v=IJquEga4-SY" tooltip="https://www.youtube.com/watch?v=IJquEga4-SY"/>
+    <hyperlink ref="G5" r:id="rId11" display="https://www.example.com/core-java-fundamentals" tooltip="https://www.example.com/core-java-fundamentals"/>
+    <hyperlink ref="J5" r:id="rId12" display="https://www.udemy.com/course/java-in-depth-become-a-complete-java-engineer" tooltip="https://www.udemy.com/course/java-in-depth-become-a-complete-java-engineer"/>
+    <hyperlink ref="L5" r:id="rId3" display="https://example.com/course-image.jpg" tooltip="https://example.com/course-image.jpg"/>
+    <hyperlink ref="O5" r:id="rId13" display="https://www.youtube.com/watch?v=eIrMbAQSU34" tooltip="https://www.youtube.com/watch?v=eIrMbAQSU34"/>
+    <hyperlink ref="G6" r:id="rId14" display="https://www.example.com/pro-c-sharp-dotnet-core" tooltip="https://www.example.com/pro-c-sharp-dotnet-core"/>
+    <hyperlink ref="J6" r:id="rId15" display="https://www.udemy.com/course/csharp-tutorial-for-beginners" tooltip="https://www.udemy.com/course/csharp-tutorial-for-beginners"/>
+    <hyperlink ref="L6" r:id="rId3" display="https://example.com/course-image.jpg" tooltip="https://example.com/course-image.jpg"/>
+    <hyperlink ref="O6" r:id="rId16" display="https://www.youtube.com/watch?v=gfkTfcpWqAY" tooltip="https://www.youtube.com/watch?v=gfkTfcpWqAY"/>
+    <hyperlink ref="G7" r:id="rId17" display="https://www.example.com/pro-aspnet-core" tooltip="https://www.example.com/pro-aspnet-core"/>
+    <hyperlink ref="J7" r:id="rId18" display="https://www.udemy.com/course/dotnet-core-mvc-for-beginners" tooltip="https://www.udemy.com/course/dotnet-core-mvc-for-beginners"/>
+    <hyperlink ref="L7" r:id="rId3" display="https://example.com/course-image.jpg" tooltip="https://example.com/course-image.jpg"/>
+    <hyperlink ref="O7" r:id="rId19" display="https://www.youtube.com/watch?v=C5cnZ-gZy2I" tooltip="https://www.youtube.com/watch?v=C5cnZ-gZy2I"/>
+    <hyperlink ref="G8" r:id="rId20" display="https://www.example.com/learning-python" tooltip="https://www.example.com/learning-python"/>
+    <hyperlink ref="J8" r:id="rId21" display="https://www.udemy.com/course/complete-python-bootcamp" tooltip="https://www.udemy.com/course/complete-python-bootcamp"/>
+    <hyperlink ref="L8" r:id="rId3" display="https://example.com/course-image.jpg" tooltip="https://example.com/course-image.jpg"/>
+    <hyperlink ref="O8" r:id="rId22" display="https://www.youtube.com/watch?v=_Z1a_9sdu4I" tooltip="https://www.youtube.com/watch?v=_Z1a_9sdu4I"/>
+    <hyperlink ref="J9" r:id="rId23" display="https://www.udemy.com/course/python-for-data-science-and-machine-learning-bootcamp" tooltip="https://www.udemy.com/course/python-for-data-science-and-machine-learning-bootcamp"/>
+    <hyperlink ref="L9" r:id="rId3" display="https://example.com/course-image.jpg" tooltip="https://example.com/course-image.jpg"/>
+    <hyperlink ref="O9" r:id="rId24" display="https://www.youtube.com/watch?v=2BrpKpWwT2A" tooltip="https://www.youtube.com/watch?v=2BrpKpWwT2A"/>
+    <hyperlink ref="G10" r:id="rId25" display="https://www.example.com/how-to-win-friends" tooltip="https://www.example.com/how-to-win-friends"/>
+    <hyperlink ref="J10" r:id="rId26" display="https://www.udemy.com/course/effective-communication-skills-course" tooltip="https://www.udemy.com/course/effective-communication-skills-course"/>
+    <hyperlink ref="L10" r:id="rId3" display="https://example.com/course-image.jpg" tooltip="https://example.com/course-image.jpg"/>
+    <hyperlink ref="O10" r:id="rId27" display="https://www.youtube.com/watch?v=6WwTakingUE" tooltip="https://www.youtube.com/watch?v=6WwTakingUE"/>
+    <hyperlink ref="G11" r:id="rId28" display="https://www.example.com/how-to-be-heard" tooltip="https://www.example.com/how-to-be-heard"/>
+    <hyperlink ref="J11" r:id="rId29" display="https://www.coursera.org/specializations/public-speaking" tooltip="https://www.coursera.org/specializations/public-speaking"/>
+    <hyperlink ref="L11" r:id="rId3" display="https://example.com/course-image.jpg" tooltip="https://example.com/course-image.jpg"/>
+    <hyperlink ref="O11" r:id="rId30" display="https://www.youtube.com/watch?v=w-HYZv6HzAs" tooltip="https://www.youtube.com/watch?v=w-HYZv6HzAs"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>